<commit_message>
update AR excel files and html files
</commit_message>
<xml_diff>
--- a/DataFiles_Excel/BubbleChart/bubble_discretionary.xlsx
+++ b/DataFiles_Excel/BubbleChart/bubble_discretionary.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\2016 Annual Report\TaggsAR2016-master\DataFiles_Excel\BubbleChart\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="13935" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -103,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,6 +136,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -166,13 +178,7 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -183,12 +189,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -517,50 +534,50 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.875" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="5" max="5" width="14.625" customWidth="1"/>
+    <col min="6" max="6" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="60" customHeight="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="3" spans="1:6" ht="28" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="8" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -580,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -600,7 +617,7 @@
         <v>3943</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -616,15 +633,15 @@
       <c r="E8" s="2">
         <v>0.01</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>735</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="2">
         <v>-0.06</v>
       </c>
       <c r="C9" s="2">
@@ -636,11 +653,11 @@
       <c r="E9" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>529</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -656,11 +673,11 @@
       <c r="E10" s="2">
         <v>0</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -676,11 +693,11 @@
       <c r="E11" s="2">
         <v>1E-3</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -700,7 +717,7 @@
         <v>4036</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -716,11 +733,11 @@
       <c r="E13" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>519</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -736,11 +753,11 @@
       <c r="E14" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>577</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -760,7 +777,7 @@
         <v>6100</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -776,11 +793,11 @@
       <c r="E16" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>619</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -793,18 +810,18 @@
       <c r="D17" s="3">
         <v>23531329699</v>
       </c>
-      <c r="E17" s="6">
-        <v>71.5</v>
+      <c r="E17" s="2">
+        <v>0.71499999999999997</v>
       </c>
       <c r="F17" s="4">
         <v>50188</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="2">
         <v>-0.09</v>
       </c>
       <c r="C18" s="2">
@@ -816,11 +833,11 @@
       <c r="E18" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>459</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -836,11 +853,11 @@
       <c r="E19" s="2">
         <v>0</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -856,11 +873,11 @@
       <c r="E20" s="2">
         <v>0</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -880,16 +897,22 @@
         <v>2438</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="10">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="C22" s="10">
+        <v>1</v>
+      </c>
       <c r="D22" s="3">
         <v>52814771803</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="10">
+        <v>1</v>
+      </c>
       <c r="F22" s="4">
         <v>70203</v>
       </c>
@@ -901,6 +924,7 @@
     <mergeCell ref="A3:F3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>